<commit_message>
Added download to AQC
</commit_message>
<xml_diff>
--- a/Data/Reportfor_Status.xlsx
+++ b/Data/Reportfor_Status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <x:si>
     <x:t>Module</x:t>
   </x:si>
@@ -473,6 +473,51 @@
   </x:si>
   <x:si>
     <x:t>18-01-2021 10:30:59 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:06:10 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:06:38 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:06:53 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:07:06 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:07:34 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:07:52 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">AQC overRide Report Download </x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:07:59 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:26:11 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:26:37 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:26:51 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:27:04 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:27:32 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:27:50 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 06:27:57 PM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -2580,6 +2625,230 @@
         <x:v>150</x:v>
       </x:c>
     </x:row>
+    <x:row r="125" spans="1:4">
+      <x:c r="A125" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B125" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C125" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D125" s="4" t="s">
+        <x:v>151</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126" spans="1:4">
+      <x:c r="A126" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B126" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C126" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D126" s="4" t="s">
+        <x:v>152</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127" spans="1:4">
+      <x:c r="A127" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B127" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C127" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D127" s="4" t="s">
+        <x:v>153</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="128" spans="1:4">
+      <x:c r="A128" s="4" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B128" s="4" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C128" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D128" s="4" t="s">
+        <x:v>154</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="129" spans="1:4">
+      <x:c r="A129" s="4" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B129" s="4" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C129" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D129" s="4" t="s">
+        <x:v>155</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="130" spans="1:4">
+      <x:c r="A130" s="4" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B130" s="4" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C130" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D130" s="4" t="s">
+        <x:v>156</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131" spans="1:4">
+      <x:c r="A131" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B131" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="C131" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D131" s="4" t="s">
+        <x:v>158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132" spans="1:4">
+      <x:c r="A132" s="4" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B132" s="4" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C132" s="4" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D132" s="4" t="s">
+        <x:v>158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133" spans="1:4">
+      <x:c r="A133" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B133" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C133" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D133" s="4" t="s">
+        <x:v>159</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134" spans="1:4">
+      <x:c r="A134" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B134" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C134" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D134" s="4" t="s">
+        <x:v>160</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135" spans="1:4">
+      <x:c r="A135" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B135" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C135" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D135" s="4" t="s">
+        <x:v>161</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136" spans="1:4">
+      <x:c r="A136" s="4" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B136" s="4" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C136" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D136" s="4" t="s">
+        <x:v>162</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="137" spans="1:4">
+      <x:c r="A137" s="4" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B137" s="4" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C137" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D137" s="4" t="s">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="138" spans="1:4">
+      <x:c r="A138" s="4" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B138" s="4" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C138" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D138" s="4" t="s">
+        <x:v>164</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" spans="1:4">
+      <x:c r="A139" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B139" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="C139" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D139" s="4" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" spans="1:4">
+      <x:c r="A140" s="4" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B140" s="4" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C140" s="4" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D140" s="4" t="s">
+        <x:v>165</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
new changes in report
</commit_message>
<xml_diff>
--- a/Data/Reportfor_Status.xlsx
+++ b/Data/Reportfor_Status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <x:si>
     <x:t>Module</x:t>
   </x:si>
@@ -518,6 +518,57 @@
   </x:si>
   <x:si>
     <x:t>22-01-2021 06:27:57 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-01-2021 10:31:03 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 11:45:30 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 11:46:04 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 11:46:19 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 11:46:31 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 11:46:59 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 11:47:14 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 11:47:20 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:42:13 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:42:43 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:44:28 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:44:59 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:45:14 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:45:27 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:45:54 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:46:13 PM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25-01-2021 12:46:20 PM</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -2849,6 +2900,258 @@
         <x:v>165</x:v>
       </x:c>
     </x:row>
+    <x:row r="141" spans="1:4">
+      <x:c r="A141" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B141" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C141" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D141" s="4" t="s">
+        <x:v>166</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142" spans="1:4">
+      <x:c r="A142" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B142" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C142" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D142" s="4" t="s">
+        <x:v>167</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143" spans="1:4">
+      <x:c r="A143" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B143" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C143" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D143" s="4" t="s">
+        <x:v>168</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144" spans="1:4">
+      <x:c r="A144" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B144" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C144" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D144" s="4" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145" spans="1:4">
+      <x:c r="A145" s="4" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B145" s="4" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C145" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D145" s="4" t="s">
+        <x:v>170</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146" spans="1:4">
+      <x:c r="A146" s="4" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B146" s="4" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C146" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D146" s="4" t="s">
+        <x:v>171</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147" spans="1:4">
+      <x:c r="A147" s="4" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B147" s="4" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C147" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D147" s="4" t="s">
+        <x:v>172</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="148" spans="1:4">
+      <x:c r="A148" s="4" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B148" s="4" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C148" s="4" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D148" s="4" t="s">
+        <x:v>173</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="149" spans="1:4">
+      <x:c r="A149" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B149" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C149" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D149" s="4" t="s">
+        <x:v>174</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="150" spans="1:4">
+      <x:c r="A150" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B150" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C150" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D150" s="4" t="s">
+        <x:v>175</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="151" spans="1:4">
+      <x:c r="A151" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B151" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C151" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D151" s="4" t="s">
+        <x:v>176</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="152" spans="1:4">
+      <x:c r="A152" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B152" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C152" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D152" s="4" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="153" spans="1:4">
+      <x:c r="A153" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B153" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C153" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D153" s="4" t="s">
+        <x:v>178</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="154" spans="1:4">
+      <x:c r="A154" s="4" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B154" s="4" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C154" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D154" s="4" t="s">
+        <x:v>179</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155" spans="1:4">
+      <x:c r="A155" s="4" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B155" s="4" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C155" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D155" s="4" t="s">
+        <x:v>180</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156" spans="1:4">
+      <x:c r="A156" s="4" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B156" s="4" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="C156" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D156" s="4" t="s">
+        <x:v>181</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157" spans="1:4">
+      <x:c r="A157" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B157" s="4" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="C157" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D157" s="4" t="s">
+        <x:v>182</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158" spans="1:4">
+      <x:c r="A158" s="4" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B158" s="4" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C158" s="4" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D158" s="4" t="s">
+        <x:v>182</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>